<commit_message>
Update conditional formatting and base readme
</commit_message>
<xml_diff>
--- a/export/v1.0.6a/biome.xlsx
+++ b/export/v1.0.6a/biome.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28702"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2025\games\microtopia\export-manual\v1.0.x\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data\2025\pwsh\MicrotopiaData\export\v1.0.6a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22466BC5-F2C6-406A-8576-DD7F0669DEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392FA7FF-3C92-4BF6-8584-8C79B4A28C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15394" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6765" yWindow="1365" windowWidth="27240" windowHeight="16950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plants" sheetId="1" r:id="rId1"/>
@@ -828,7 +828,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -846,6 +846,12 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -876,9 +882,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -887,21 +892,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -911,29 +910,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1017,13 +993,239 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1065,11 +1267,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CBB0FE41-59A3-4D72-8A16-E61EE74D812C}" name="Biome_Objects" displayName="Biome_Objects" ref="A1:L80" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CBB0FE41-59A3-4D72-8A16-E61EE74D812C}" name="Biome_Objects" displayName="Biome_Objects" ref="A1:L80" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="A1:L80" xr:uid="{CBB0FE41-59A3-4D72-8A16-E61EE74D812C}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{D72E30D4-0710-41C4-884B-8CAB96B1E0F4}" name="CODE"/>
-    <tableColumn id="2" xr3:uid="{D0D1CCB7-31F3-4DC8-8EC3-FB6633D72BBC}" name="TITLE" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{D0D1CCB7-31F3-4DC8-8EC3-FB6633D72BBC}" name="TITLE" dataDxfId="33"/>
     <tableColumn id="3" xr3:uid="{340B2C87-821A-4611-9E1B-4C57E8D0B5FF}" name="DESCRIPTION"/>
     <tableColumn id="4" xr3:uid="{C04D5471-237F-44DE-B910-A436C87022DF}" name="UNCLICKABLE"/>
     <tableColumn id="5" xr3:uid="{22232B06-25BF-4E4E-B983-1050AEC407A2}" name="TRAILS PASS THROUGH"/>
@@ -1404,37 +1606,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.61328125" customWidth="1"/>
-    <col min="2" max="2" width="19.69140625" customWidth="1"/>
-    <col min="3" max="3" width="15.07421875" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.07421875" customWidth="1"/>
-    <col min="6" max="6" width="14.4609375" customWidth="1"/>
-    <col min="7" max="7" width="16.4609375" customWidth="1"/>
-    <col min="8" max="8" width="17.23046875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="13.53515625" customWidth="1"/>
-    <col min="11" max="11" width="12.4609375" customWidth="1"/>
-    <col min="12" max="12" width="16.69140625" customWidth="1"/>
-    <col min="13" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="25.15234375" customWidth="1"/>
-    <col min="15" max="15" width="13.84375" customWidth="1"/>
-    <col min="16" max="16" width="14.3046875" customWidth="1"/>
-    <col min="17" max="17" width="17.4609375" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.3" x14ac:dyDescent="0.75">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1487,58 +1689,58 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="49.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:17" ht="49.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1585,7 +1787,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1632,7 +1834,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1679,7 +1881,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1726,7 +1928,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1773,7 +1975,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1823,7 +2025,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1873,7 +2075,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1923,7 +2125,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1970,7 +2172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2017,7 +2219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2064,7 +2266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2111,7 +2313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -2158,7 +2360,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2205,7 +2407,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2252,7 +2454,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2299,7 +2501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2346,7 +2548,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2393,7 +2595,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -2440,7 +2642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2487,7 +2689,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -2506,7 +2708,7 @@
       <c r="F27">
         <v>3600</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="6">
         <v>999999</v>
       </c>
       <c r="H27">
@@ -2537,7 +2739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2556,7 +2758,7 @@
       <c r="F28">
         <v>3600</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="6">
         <v>999999</v>
       </c>
       <c r="H28">
@@ -2588,50 +2790,17 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P3:P28">
-    <cfRule type="dataBar" priority="11">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6D22CE3C-9F45-49E4-83A6-052BA844294A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O28">
-    <cfRule type="dataBar" priority="10">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AB526BC1-8BE8-4BB0-8902-E5CCE60274EF}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q28">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A3:Q28">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="17" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B28">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
+        <color rgb="FF63C384"/>
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
@@ -2641,15 +2810,160 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C28">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F72F3DFC-EE93-4575-BFC1-D9BA219B2BC2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O28">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AB526BC1-8BE8-4BB0-8902-E5CCE60274EF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P28">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
+        <color rgb="FF63C384"/>
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F72F3DFC-EE93-4575-BFC1-D9BA219B2BC2}</x14:id>
+          <x14:id>{6D22CE3C-9F45-49E4-83A6-052BA844294A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q28">
+    <cfRule type="cellIs" dxfId="2" priority="18" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:E28">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{13286A32-284B-4ADE-B198-7B39DA3FA34B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F28">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{661C0F74-928C-4AA8-906B-985557E9C12A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G25">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1CC4AFF9-9905-4A1B-91FD-23E6C2FB015A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H28">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{12132401-9683-4D4E-82A6-A3925A6516B0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J28">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5A01CCE3-FE8C-4195-8859-173F1F36197E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K28">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8D3CCB5C-E004-4011-9F55-8D4C8078C91F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M28">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{79DCDF15-4F87-4218-888D-257DA50DEF2A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N28">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A1DCDBF2-E58A-44C7-8980-3583B767A3D0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2662,28 +2976,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6D22CE3C-9F45-49E4-83A6-052BA844294A}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>P3:P28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{AB526BC1-8BE8-4BB0-8902-E5CCE60274EF}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>O3:O28</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FE2C1A81-A0E0-4589-9FDC-920F096F5631}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
@@ -2706,6 +2998,116 @@
           </x14:cfRule>
           <xm:sqref>C3:C28</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AB526BC1-8BE8-4BB0-8902-E5CCE60274EF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O3:O28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6D22CE3C-9F45-49E4-83A6-052BA844294A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P3:P28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{13286A32-284B-4ADE-B198-7B39DA3FA34B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D3:E28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{661C0F74-928C-4AA8-906B-985557E9C12A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F3:F28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1CC4AFF9-9905-4A1B-91FD-23E6C2FB015A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G4:G25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{12132401-9683-4D4E-82A6-A3925A6516B0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H3:H28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5A01CCE3-FE8C-4195-8859-173F1F36197E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J3:J28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8D3CCB5C-E004-4011-9F55-8D4C8078C91F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3:K28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{79DCDF15-4F87-4218-888D-257DA50DEF2A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A1DCDBF2-E58A-44C7-8980-3583B767A3D0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N3:N28</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -2716,100 +3118,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678FB375-6C30-42FA-9228-D07C22FF2E9D}">
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="K15" sqref="K14:K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.921875" customWidth="1"/>
-    <col min="4" max="5" width="1.921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.07421875" customWidth="1"/>
-    <col min="8" max="8" width="12.921875" customWidth="1"/>
-    <col min="9" max="9" width="13.3046875" customWidth="1"/>
-    <col min="10" max="10" width="13.07421875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.84375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -2832,11 +3235,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E6" t="s">
@@ -2855,11 +3258,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E7" t="s">
@@ -2875,11 +3278,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>82</v>
       </c>
       <c r="E8" t="s">
@@ -2895,11 +3298,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E9" t="s">
@@ -2915,7 +3318,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2935,11 +3338,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E11" t="s">
@@ -2958,11 +3361,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E12" t="s">
@@ -2981,11 +3384,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E13" t="s">
@@ -3004,11 +3407,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E14" t="s">
@@ -3027,11 +3430,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E15" t="s">
@@ -3047,7 +3450,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -3064,7 +3467,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -3074,18 +3477,18 @@
       <c r="F17" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>101</v>
       </c>
       <c r="K17" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F18" t="s">
@@ -3098,7 +3501,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -3115,7 +3518,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -3138,7 +3541,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -3158,7 +3561,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3178,7 +3581,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -3198,11 +3601,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>119</v>
       </c>
       <c r="E24" t="s">
@@ -3218,11 +3621,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E25" t="s">
@@ -3235,7 +3638,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -3258,7 +3661,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -3281,27 +3684,27 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E30" t="s">
@@ -3311,7 +3714,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -3325,7 +3728,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>138</v>
       </c>
@@ -3339,11 +3742,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E33" t="s">
@@ -3356,7 +3759,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -3370,7 +3773,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -3384,23 +3787,23 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3417,7 +3820,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -3427,18 +3830,18 @@
       <c r="F39" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>101</v>
       </c>
       <c r="K39" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F40" t="s">
@@ -3451,27 +3854,27 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-    </row>
-    <row r="43" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>157</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F43" t="s">
@@ -3487,11 +3890,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F44" t="s">
@@ -3507,11 +3910,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>166</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>167</v>
       </c>
       <c r="F45" t="s">
@@ -3527,7 +3930,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>170</v>
       </c>
@@ -3547,27 +3950,27 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-    </row>
-    <row r="49" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>175</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F49" t="s">
@@ -3583,11 +3986,11 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F50" t="s">
@@ -3603,11 +4006,11 @@
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>181</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F51" t="s">
@@ -3623,7 +4026,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>184</v>
       </c>
@@ -3643,11 +4046,11 @@
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>187</v>
       </c>
       <c r="F53" t="s">
@@ -3663,11 +4066,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>190</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>191</v>
       </c>
       <c r="F54" t="s">
@@ -3683,11 +4086,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>194</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>191</v>
       </c>
       <c r="F55" t="s">
@@ -3703,7 +4106,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>197</v>
       </c>
@@ -3726,11 +4129,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>201</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>202</v>
       </c>
       <c r="F57" t="s">
@@ -3746,11 +4149,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>205</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>202</v>
       </c>
       <c r="F58" t="s">
@@ -3766,7 +4169,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>208</v>
       </c>
@@ -3786,7 +4189,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>212</v>
       </c>
@@ -3806,7 +4209,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>216</v>
       </c>
@@ -3826,7 +4229,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>220</v>
       </c>
@@ -3836,7 +4239,7 @@
       <c r="F62" t="s">
         <v>125</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="2" t="s">
         <v>222</v>
       </c>
       <c r="I62">
@@ -3846,27 +4249,27 @@
         <v>223</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-    </row>
-    <row r="65" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+    </row>
+    <row r="65" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>225</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>226</v>
       </c>
       <c r="F65" t="s">
@@ -3882,7 +4285,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -3905,7 +4308,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -3928,7 +4331,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>233</v>
       </c>
@@ -3951,7 +4354,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>235</v>
       </c>
@@ -3974,11 +4377,11 @@
         <v>236</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>237</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D70" t="s">
@@ -3991,11 +4394,11 @@
         <v>238</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>239</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D71" t="s">
@@ -4008,11 +4411,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>241</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D72" t="s">
@@ -4025,11 +4428,11 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>243</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D73" t="s">
@@ -4042,11 +4445,11 @@
         <v>244</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>245</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D74" t="s">
@@ -4059,11 +4462,11 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>247</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D75" t="s">
@@ -4076,11 +4479,11 @@
         <v>248</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>249</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D76" t="s">
@@ -4093,11 +4496,11 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>251</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D77" t="s">
@@ -4107,11 +4510,11 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>253</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D78" t="s">
@@ -4121,11 +4524,11 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>255</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D79" t="s">
@@ -4135,11 +4538,11 @@
         <v>256</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>257</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>226</v>
       </c>
       <c r="D80" t="s">
@@ -4150,24 +4553,55 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:I80">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="A2:A80">
+    <cfRule type="expression" dxfId="31" priority="2">
+      <formula>"// plants"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:L80">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:L80">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="H2:I80">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A80">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>"// plants"</formula>
+  <conditionalFormatting sqref="I2:I80">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C7859DF5-6DAC-4FC4-AE51-8F8DD34CFBC1}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C7859DF5-6DAC-4FC4-AE51-8F8DD34CFBC1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I2:I80</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>